<commit_message>
Update the course information of iSchool
</commit_message>
<xml_diff>
--- a/Course List.xlsx
+++ b/Course List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Friday" sheetId="5" r:id="rId5"/>
     <sheet name="legends" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
   <si>
     <t>Time</t>
   </si>
@@ -93,13 +93,16 @@
   </si>
   <si>
     <t>17:30-18:30</t>
+  </si>
+  <si>
+    <t>SUM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,12 +127,6 @@
     <font>
       <sz val="11"/>
       <color theme="4"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -176,7 +173,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -458,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -517,14 +513,12 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="7">
-        <v>28</v>
-      </c>
+      <c r="B2" s="6"/>
       <c r="C2" s="4">
         <v>16</v>
       </c>
-      <c r="D2">
-        <v>111</v>
+      <c r="D2" s="4">
+        <v>5</v>
       </c>
       <c r="G2" s="4">
         <v>51</v>
@@ -541,7 +535,7 @@
         <v>46</v>
       </c>
       <c r="D3" s="4">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G3" s="4">
         <v>24</v>
@@ -551,11 +545,31 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="D4" s="4">
-        <v>9</v>
-      </c>
+      <c r="D4" s="4"/>
       <c r="G4" s="4">
         <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4">
+        <f>SUM(C2:C3)</f>
+        <v>62</v>
+      </c>
+      <c r="D9" s="4">
+        <v>14</v>
+      </c>
+      <c r="G9" s="4">
+        <f>SUM(G2:G4)</f>
+        <v>84</v>
+      </c>
+      <c r="I9" s="3">
+        <v>9</v>
+      </c>
+      <c r="J9" s="4">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -565,10 +579,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -626,7 +640,7 @@
       <c r="C2" s="4">
         <v>26</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>29</v>
       </c>
       <c r="J2" s="4">
@@ -637,18 +651,16 @@
       <c r="C3" s="4">
         <v>56</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>25</v>
       </c>
-      <c r="J3" s="4">
-        <v>31</v>
-      </c>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="C4" s="4">
         <v>16</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>21</v>
       </c>
       <c r="J4" s="3">
@@ -663,6 +675,31 @@
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="G6" s="4">
         <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4">
+        <f>SUM(C2:C4)</f>
+        <v>98</v>
+      </c>
+      <c r="G9" s="6">
+        <f>SUM(G2:G4)</f>
+        <v>75</v>
+      </c>
+      <c r="J9" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G10" s="4">
+        <f>SUM(G5:G6)</f>
+        <v>56</v>
+      </c>
+      <c r="J10" s="3">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -672,17 +709,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="11" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.3984375" style="8" customWidth="1"/>
+    <col min="12" max="12" width="10.3984375" style="7" customWidth="1"/>
     <col min="13" max="15" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -720,7 +757,7 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="M1" t="s">
@@ -734,22 +771,17 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B2" s="7">
-        <v>28</v>
-      </c>
+      <c r="B2" s="6"/>
       <c r="C2" s="3">
         <v>25</v>
       </c>
-      <c r="D2">
-        <v>111</v>
-      </c>
       <c r="E2" s="3">
         <v>7</v>
       </c>
       <c r="F2" s="4">
         <v>25</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>17</v>
       </c>
       <c r="I2" s="3">
@@ -763,13 +795,47 @@
       <c r="D3" s="3">
         <v>19</v>
       </c>
-      <c r="G3" s="6">
-        <v>7</v>
+      <c r="G3" s="4">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D4" s="4">
         <v>21</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3">
+        <v>19</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4">
+        <v>25</v>
+      </c>
+      <c r="G9" s="4">
+        <v>34</v>
+      </c>
+      <c r="I9" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="D10" s="4">
+        <v>21</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -779,10 +845,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A9" sqref="A9:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -886,6 +952,36 @@
         <v>23</v>
       </c>
     </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4">
+        <f>SUM(C2:C7)</f>
+        <v>77</v>
+      </c>
+      <c r="F9" s="4">
+        <v>18</v>
+      </c>
+      <c r="G9" s="3">
+        <f>SUM(G2:G3)</f>
+        <v>53</v>
+      </c>
+      <c r="H9" s="3">
+        <v>23</v>
+      </c>
+      <c r="I9" s="3">
+        <v>21</v>
+      </c>
+      <c r="L9" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G10" s="4">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -893,10 +989,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -979,6 +1075,24 @@
         <v>27</v>
       </c>
     </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4">
+        <f>SUM(C2:C5)</f>
+        <v>88</v>
+      </c>
+      <c r="G9" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G10" s="4">
+        <f>SUM(G4,G2)</f>
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -988,7 +1102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>